<commit_message>
All 2 generic and 4 Voortoets cross section models ready.
</commit_message>
<xml_diff>
--- a/Projects/VoortoetsAGT/cases/ZwaerteVallei/ZwaerteVallei.xlsx
+++ b/Projects/VoortoetsAGT/cases/ZwaerteVallei/ZwaerteVallei.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/VoortoetsAGT/cases/ZwaerteVallei/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E493C1-E850-1F43-A4A2-7C15E0F8BFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8009A552-AC46-6441-80DB-AFB586723262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9460" yWindow="-22740" windowWidth="30600" windowHeight="19860" tabRatio="751" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9460" yWindow="-22740" windowWidth="30600" windowHeight="19860" tabRatio="751" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAM" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -95,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -109,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -122,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000005000000}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1473,9 +1473,6 @@
     <t>darkviolet</t>
   </si>
   <si>
-    <t>Years</t>
-  </si>
-  <si>
     <t>cyan</t>
   </si>
   <si>
@@ -1483,6 +1480,9 @@
   </si>
   <si>
     <t>NEWTON UNDER_RELAXATION</t>
+  </si>
+  <si>
+    <t>Zero-based</t>
   </si>
 </sst>
 </file>
@@ -3595,7 +3595,7 @@
   <dimension ref="A1:H477"/>
   <sheetViews>
     <sheetView topLeftCell="A200" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="C219" sqref="C219"/>
+      <selection activeCell="C218" sqref="C218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3720,7 +3720,7 @@
         <v>110</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>383</v>
@@ -5879,7 +5879,7 @@
         <v>45</v>
       </c>
       <c r="C218" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.15">
@@ -11886,18 +11886,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="264" zoomScaleNormal="264" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -11905,42 +11911,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="14">
         <v>45292</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="9">
+        <f>DATE(2054,1,1)-DATE(2024,1,1)</f>
+        <v>10958</v>
+      </c>
+      <c r="D3" s="9">
         <v>30</v>
       </c>
-      <c r="D3" s="9">
-        <f>C3*365.25</f>
-        <v>10957.5</v>
-      </c>
       <c r="E3" s="9">
-        <v>30</v>
+        <v>1.25</v>
       </c>
       <c r="F3" s="9">
-        <v>1.25</v>
-      </c>
-      <c r="G3" s="9">
         <v>1</v>
       </c>
     </row>
@@ -11956,7 +11956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="237" zoomScaleNormal="237" workbookViewId="0">
+    <sheetView zoomScale="237" zoomScaleNormal="237" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -12247,7 +12247,7 @@
         <v>1E-4</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>392</v>

</xml_diff>